<commit_message>
add the project automation
</commit_message>
<xml_diff>
--- a/Tese Cases for Ecommerce project.xlsx
+++ b/Tese Cases for Ecommerce project.xlsx
@@ -1235,7 +1235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1246,14 +1246,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1286,9 +1280,6 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1296,10 +1287,16 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1582,20 +1579,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56" style="7" customWidth="1"/>
-    <col min="3" max="3" width="81.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="60.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="70.7109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="22" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="9"/>
+    <col min="2" max="2" width="56" style="5" customWidth="1"/>
+    <col min="3" max="3" width="81.7109375" style="22" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="70.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="22" style="5" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1605,7 +1602,7 @@
       <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -1621,24 +1618,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" s="6" customFormat="1" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="E2" s="5"/>
+      <c r="F2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1646,19 +1643,19 @@
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1666,19 +1663,19 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1686,22 +1683,22 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1709,22 +1706,22 @@
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1732,22 +1729,22 @@
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1758,19 +1755,19 @@
       <c r="B8" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1778,22 +1775,22 @@
       <c r="A9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="7" t="s">
+      <c r="F9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1801,22 +1798,22 @@
       <c r="A10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="F10" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1824,22 +1821,22 @@
       <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="7" t="s">
+      <c r="F11" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1847,19 +1844,19 @@
       <c r="A12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="7" t="s">
+      <c r="F12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1867,22 +1864,22 @@
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="7" t="s">
+      <c r="F13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1890,22 +1887,22 @@
       <c r="A14" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="7" t="s">
+      <c r="F14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1913,22 +1910,22 @@
       <c r="A15" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="F15" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="7" t="s">
+      <c r="F15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1936,22 +1933,22 @@
       <c r="A16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="7" t="s">
+      <c r="F16" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1959,22 +1956,22 @@
       <c r="A17" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="7" t="s">
+      <c r="F17" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1982,22 +1979,22 @@
       <c r="A18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="F18" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="7" t="s">
+      <c r="F18" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2005,22 +2002,22 @@
       <c r="A19" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="13" t="s">
         <v>125</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2028,22 +2025,22 @@
       <c r="A20" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="F20" s="12" t="s">
+      <c r="F20" s="10" t="s">
         <v>128</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2051,22 +2048,22 @@
       <c r="A21" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="F21" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="7" t="s">
+      <c r="F21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2074,19 +2071,19 @@
       <c r="A22" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="7" t="s">
+      <c r="F22" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2094,22 +2091,22 @@
       <c r="A23" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F23" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="7" t="s">
+      <c r="F23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2117,22 +2114,22 @@
       <c r="A24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F24" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="7" t="s">
+      <c r="F24" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2140,22 +2137,22 @@
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="13" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="F25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="7" t="s">
+      <c r="F25" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2163,22 +2160,22 @@
       <c r="A26" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E26" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F26" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="7" t="s">
+      <c r="F26" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2186,54 +2183,54 @@
       <c r="A27" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="F27" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="7" t="s">
+      <c r="F27" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="19" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="17"/>
-      <c r="G28" s="17"/>
+    <row r="28" spans="1:7" s="16" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="13" t="s">
         <v>161</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="F29" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="7" t="s">
+      <c r="F29" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2241,22 +2238,22 @@
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E30" s="5" t="s">
+      <c r="E30" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="7" t="s">
+      <c r="F30" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2264,22 +2261,22 @@
       <c r="A31" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E31" s="5" t="s">
+      <c r="E31" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="F31" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="7" t="s">
+      <c r="F31" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="5" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2287,22 +2284,22 @@
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="13" t="s">
         <v>174</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="G32" s="5" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2310,56 +2307,56 @@
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="F33" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="7" t="s">
+      <c r="F33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="23" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="22"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="21"/>
+    <row r="34" spans="1:7" s="19" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="18"/>
     </row>
     <row r="35" spans="1:7" ht="208.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="F35" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="7" t="s">
+      <c r="F35" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2367,22 +2364,22 @@
       <c r="A36" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="F36" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="7" t="s">
+      <c r="F36" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2390,22 +2387,22 @@
       <c r="A37" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="F37" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="7" t="s">
+      <c r="F37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2413,22 +2410,22 @@
       <c r="A38" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="C38" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E38" s="14" t="s">
+      <c r="E38" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="F38" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38" s="7" t="s">
+      <c r="F38" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2436,22 +2433,22 @@
       <c r="A39" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="F39" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="7" t="s">
+      <c r="F39" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2459,22 +2456,22 @@
       <c r="A40" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="F40" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="7" t="s">
+      <c r="F40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2482,22 +2479,22 @@
       <c r="A41" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="13" t="s">
         <v>208</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="F41" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="7" t="s">
+      <c r="F41" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2505,22 +2502,22 @@
       <c r="A42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E42" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="F42" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="7" t="s">
+      <c r="F42" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2528,22 +2525,22 @@
       <c r="A43" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="13" t="s">
         <v>216</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="E43" s="5" t="s">
+      <c r="E43" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2551,22 +2548,22 @@
       <c r="A44" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="E44" s="5" t="s">
+      <c r="E44" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="F44" s="12" t="s">
+      <c r="F44" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="5" t="s">
         <v>194</v>
       </c>
     </row>
@@ -2574,22 +2571,22 @@
       <c r="A45" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="C45" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E45" s="5" t="s">
+      <c r="E45" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="F45" s="12" t="s">
+      <c r="F45" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="G45" s="5" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>